<commit_message>
fixes #6 and #5
</commit_message>
<xml_diff>
--- a/DOC/Temporizador_v8 - Gastos.xlsx
+++ b/DOC/Temporizador_v8 - Gastos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcelo\Desktop\Temporizador\TemporizadorAC\DOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B16AFF-8C5B-4278-BF1A-DAE9D3D93991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB903CC-5BCD-420A-A51A-DF4BB438BAB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -571,14 +571,14 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C4" s="1">
         <v>20</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -601,14 +601,14 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>2.5499999999999998</v>
+        <v>0.2</v>
       </c>
       <c r="C6" s="1">
         <v>200</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="0"/>
-        <v>509.99999999999994</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -725,11 +725,11 @@
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D14" s="6">
         <f>SUM(D2:D13)</f>
-        <v>984.49</v>
+        <v>414.49</v>
       </c>
       <c r="E14" s="1">
         <f>D14/10</f>
-        <v>98.448999999999998</v>
+        <v>41.448999999999998</v>
       </c>
       <c r="F14" s="6">
         <v>70</v>
@@ -777,12 +777,15 @@
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="B18" s="1">
+        <v>-40</v>
+      </c>
       <c r="C18" s="1">
         <v>1</v>
       </c>
       <c r="D18" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-40</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -854,11 +857,11 @@
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D26" s="6">
         <f>SUM(D16:D25)</f>
-        <v>-520</v>
+        <v>-560</v>
       </c>
       <c r="E26" s="1">
         <f>-D26/F14</f>
-        <v>7.4285714285714288</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>